<commit_message>
Tested Execution, Fixed Some Bugs and Warnings. Works well : D (still no forwarding)
</commit_message>
<xml_diff>
--- a/Execute/Exec Tests sheet.xlsx
+++ b/Execute/Exec Tests sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A\CA\project\ar-kak-tecture\Execute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C07E4976-6B21-41A1-B288-D137AA9B6ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C3D3FD-A50B-4482-9B7C-5E088F1D7763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E795A3FC-67AE-4511-B765-0554307C1292}"/>
+    <workbookView xWindow="15540" yWindow="1788" windowWidth="7500" windowHeight="7488" xr2:uid="{E795A3FC-67AE-4511-B765-0554307C1292}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>opcode</t>
   </si>
@@ -145,6 +145,123 @@
   </si>
   <si>
     <t>11111'</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>SETC</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>LDD</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>LDM</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>JZ</t>
+  </si>
+  <si>
+    <t>JN</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>RTI</t>
+  </si>
+  <si>
+    <t>x"0000"</t>
+  </si>
+  <si>
+    <t>x"FFFF"</t>
+  </si>
+  <si>
+    <t>IADD</t>
+  </si>
+  <si>
+    <t>x"F24A"</t>
+  </si>
+  <si>
+    <t>x"1244"</t>
+  </si>
+  <si>
+    <t>x"1234"</t>
+  </si>
+  <si>
+    <t>x"3DEF"</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x"FFFE"</t>
+  </si>
+  <si>
+    <t>x"5023"</t>
+  </si>
+  <si>
+    <t>x"1240"</t>
+  </si>
+  <si>
+    <t>x"E494"</t>
+  </si>
+  <si>
+    <t>x"0001"</t>
+  </si>
+  <si>
+    <t>x"2BBB"</t>
   </si>
 </sst>
 </file>
@@ -283,9 +400,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,9 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -310,6 +423,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,219 +753,790 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5109640C-ADAB-480D-A756-F772DE7EC3CB}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" customWidth="1"/>
-    <col min="7" max="7" width="3.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" customWidth="1"/>
+    <col min="7" max="7" width="4.77734375" customWidth="1"/>
+    <col min="8" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" customWidth="1"/>
+    <col min="14" max="14" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="B8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="B9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="B13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="B14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="B15" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+      <c r="B16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+      <c r="B17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+      <c r="B18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="B20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="B21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="B22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="B23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="B24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="B25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="B26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="B27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G27" s="2"/>
+      <c r="B28" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated xDDDDDDDDDDDDDDDDDD lol haha
</commit_message>
<xml_diff>
--- a/Execute/Exec Tests sheet.xlsx
+++ b/Execute/Exec Tests sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A\CA\project\ar-kak-tecture\Execute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C3D3FD-A50B-4482-9B7C-5E088F1D7763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750F4FC9-9C5E-4AA7-9155-F232525231D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="1788" windowWidth="7500" windowHeight="7488" xr2:uid="{E795A3FC-67AE-4511-B765-0554307C1292}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E795A3FC-67AE-4511-B765-0554307C1292}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5109640C-ADAB-480D-A756-F772DE7EC3CB}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>

</xml_diff>